<commit_message>
DOCUMENTATION: Modify the HFM format
</commit_message>
<xml_diff>
--- a/documentation/Halfling Model File format.xlsx
+++ b/documentation/Halfling Model File format.xlsx
@@ -363,7 +363,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -375,13 +375,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -677,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
DOCUMENTATION: Moved the string table and removed InputDesc
TODO: Move this to an ASCII table so it can be more easily seen by Git
</commit_message>
<xml_diff>
--- a/documentation/Halfling Model File format.xlsx
+++ b/documentation/Halfling Model File format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
   <si>
     <t>Halfling Model File format</t>
   </si>
@@ -219,30 +219,15 @@
     <t>F</t>
   </si>
   <si>
-    <t>String Table Offset</t>
-  </si>
-  <si>
     <t>String Table</t>
   </si>
   <si>
-    <t xml:space="preserve">        String length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        String</t>
-  </si>
-  <si>
     <t>char[]</t>
   </si>
   <si>
-    <t>Offset from the start of this file to the string table. Is NULL if the table doesn't exist</t>
-  </si>
-  <si>
     <t>Length of the string</t>
   </si>
   <si>
-    <t>The string data. DOES NOT HAVE A NULL TERMINATION</t>
-  </si>
-  <si>
     <t>int32</t>
   </si>
   <si>
@@ -280,6 +265,30 @@
   </si>
   <si>
     <t>The Specular Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Num strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        String data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                String length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                String</t>
+  </si>
+  <si>
+    <t>The number of strings in the table</t>
+  </si>
+  <si>
+    <t>The string characters. DOES NOT HAVE A NULL TERMINATION</t>
+  </si>
+  <si>
+    <t>HAS_STRING_TABLE</t>
+  </si>
+  <si>
+    <t>0x0008</t>
   </si>
 </sst>
 </file>
@@ -668,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -765,423 +774,437 @@
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
+      <c r="C9" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
+      <c r="D22" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C43" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C121">
+  <conditionalFormatting sqref="C5:C123">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C5)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
DOCS: Update HMF docs regarding the removal of ambient color and spec intensity
</commit_message>
<xml_diff>
--- a/documentation/Halfling Model File format.xlsx
+++ b/documentation/Halfling Model File format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
   <si>
     <t>Halfling Model File format</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Subset[]</t>
   </si>
   <si>
-    <t xml:space="preserve">        Material Ambient Color</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Material Diffuse Color</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>float[3]</t>
   </si>
   <si>
-    <t xml:space="preserve">        Material Specular Intensity</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -252,13 +246,7 @@
     <t>The number of indices used by the subset (All used indices must be in the range IndexStart + IndexCount)</t>
   </si>
   <si>
-    <t>The RGB ambient color values of the material</t>
-  </si>
-  <si>
     <t>The RGBA diffuse color values of the material</t>
-  </si>
-  <si>
-    <t>The Specular Intensity</t>
   </si>
   <si>
     <t>The RGB specular color values of the material</t>
@@ -677,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -729,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -749,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -769,74 +757,74 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -847,7 +835,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -861,7 +849,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
@@ -875,7 +863,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -889,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>29</v>
@@ -903,7 +891,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
@@ -917,7 +905,7 @@
         <v>24</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>28</v>
@@ -931,7 +919,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>38</v>
@@ -945,7 +933,7 @@
         <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>39</v>
@@ -959,7 +947,7 @@
         <v>37</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -973,7 +961,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>43</v>
@@ -987,7 +975,7 @@
         <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>49</v>
@@ -1001,10 +989,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1015,10 +1003,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1029,10 +1017,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1043,10 +1031,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1054,41 +1042,41 @@
         <v>51</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1096,41 +1084,41 @@
         <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1138,73 +1126,45 @@
         <v>60</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C123">
+  <conditionalFormatting sqref="C5:C121">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C5)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
COMMON: Remove instance data from the HMF format
Instance data should be stored in the scene, not with the model.
</commit_message>
<xml_diff>
--- a/documentation/Halfling Model File format.xlsx
+++ b/documentation/Halfling Model File format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Halfling Model File format</t>
   </si>
@@ -96,15 +96,9 @@
     <t>Index Buffer Desc</t>
   </si>
   <si>
-    <t>Instance Buffer Desc</t>
-  </si>
-  <si>
     <t xml:space="preserve">A hard cast of the index buffer description </t>
   </si>
   <si>
-    <t xml:space="preserve">A hard cast of the instance buffer description </t>
-  </si>
-  <si>
     <t>A hard cast of the vertex buffer description</t>
   </si>
   <si>
@@ -114,21 +108,6 @@
     <t>Index data</t>
   </si>
   <si>
-    <t>Instance buffer data</t>
-  </si>
-  <si>
-    <t>HAS_INSTANCE_BUFFER</t>
-  </si>
-  <si>
-    <t>0x0002</t>
-  </si>
-  <si>
-    <t>HAS_INSTANCE_BUFFER_DATA</t>
-  </si>
-  <si>
-    <t>0x0004</t>
-  </si>
-  <si>
     <t>void[]</t>
   </si>
   <si>
@@ -138,12 +117,6 @@
     <t>Will be read in a single block using IndexBufferDesc.ByteWidth</t>
   </si>
   <si>
-    <t>Will be read in a single block using InstanceBufferDesc.ByteWidth</t>
-  </si>
-  <si>
-    <t>Version 1</t>
-  </si>
-  <si>
     <t>Num Subsets</t>
   </si>
   <si>
@@ -276,7 +249,10 @@
     <t>HAS_STRING_TABLE</t>
   </si>
   <si>
-    <t>0x0008</t>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <t>0x0001</t>
   </si>
 </sst>
 </file>
@@ -665,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -688,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
@@ -717,16 +693,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -737,16 +713,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -757,74 +727,68 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -835,7 +799,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -849,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
@@ -863,7 +827,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -877,10 +841,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -891,280 +855,252 @@
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="C39" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>71</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C121">
+  <conditionalFormatting sqref="C5:C119">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C5)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
DOCUMENTATION: Create a new HMF format to support the new material system
</commit_message>
<xml_diff>
--- a/documentation/Halfling Model File format.xlsx
+++ b/documentation/Halfling Model File format.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Halfling Model File format</t>
   </si>
@@ -144,42 +144,6 @@
     <t>Subset[]</t>
   </si>
   <si>
-    <t xml:space="preserve">        Material Diffuse Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Material Specular Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Diffuse Color Map Filename</t>
-  </si>
-  <si>
-    <t>float[4]</t>
-  </si>
-  <si>
-    <t>float[3]</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Material Specular Power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Specular Color Map Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Specular Power Map Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Alpha Map Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Normal Map Filename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Bump Map Filename</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -195,18 +159,6 @@
     <t>Length of the string</t>
   </si>
   <si>
-    <t>int32</t>
-  </si>
-  <si>
-    <t>An index to the string table. -1 if it doesn't exist.</t>
-  </si>
-  <si>
-    <t>An index to the string table. -1 if it doesn't exist. Mutually exclusive with Normal Map</t>
-  </si>
-  <si>
-    <t>An index to the string table. -1 if it doesn't exist. Mutually exclusive with Bump Map</t>
-  </si>
-  <si>
     <t>The index to the first vertex used by the subset</t>
   </si>
   <si>
@@ -219,15 +171,6 @@
     <t>The number of indices used by the subset (All used indices must be in the range IndexStart + IndexCount)</t>
   </si>
   <si>
-    <t>The RGBA diffuse color values of the material</t>
-  </si>
-  <si>
-    <t>The RGB specular color values of the material</t>
-  </si>
-  <si>
-    <t>The Specular Power</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Num strings</t>
   </si>
   <si>
@@ -249,10 +192,94 @@
     <t>HAS_STRING_TABLE</t>
   </si>
   <si>
-    <t>Version 2</t>
-  </si>
-  <si>
     <t>0x0001</t>
+  </si>
+  <si>
+    <t>Version 3</t>
+  </si>
+  <si>
+    <t>Sampling Enum</t>
+  </si>
+  <si>
+    <t>An enum from Sampling Enum</t>
+  </si>
+  <si>
+    <t>LINEAR_WRAP</t>
+  </si>
+  <si>
+    <t>LINEAR_CLAMP</t>
+  </si>
+  <si>
+    <t>LINEAR_BORDER</t>
+  </si>
+  <si>
+    <t>POINT_CLAMP</t>
+  </si>
+  <si>
+    <t>POINT_WRAP</t>
+  </si>
+  <si>
+    <t>ANISOTROPIC_WRAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        AABB_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        AABB_max</t>
+  </si>
+  <si>
+    <t>float3</t>
+  </si>
+  <si>
+    <t>The minimum bounds of the AABB surrounding the subset</t>
+  </si>
+  <si>
+    <t>The maximum bounds of the AABB surrounding the subset</t>
+  </si>
+  <si>
+    <t>An index to the string table</t>
+  </si>
+  <si>
+    <t>The number of textures in the table</t>
+  </si>
+  <si>
+    <t>0x0002</t>
+  </si>
+  <si>
+    <t>Material Table</t>
+  </si>
+  <si>
+    <t>An index to the material table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Num Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Material data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Material HMAT FilePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Num textures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Texture data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        FilePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        Sampler</t>
+  </si>
+  <si>
+    <t>The number of materials in the table</t>
+  </si>
+  <si>
+    <t>HAS_MATERIAL_TABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Material Index</t>
   </si>
 </sst>
 </file>
@@ -317,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,6 +359,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,15 +669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="96" style="1" customWidth="1"/>
@@ -664,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1">
@@ -693,16 +719,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -713,10 +739,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -727,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
@@ -735,60 +767,69 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickBot="1">
+      <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="F14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -799,10 +840,16 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -813,13 +860,27 @@
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -827,13 +888,27 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="F19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -841,13 +916,13 @@
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -855,13 +930,13 @@
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -869,13 +944,13 @@
         <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -883,224 +958,244 @@
         <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="B41" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>62</v>
+      <c r="B42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C119">
+  <conditionalFormatting sqref="C5:C124">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C5)))</formula>
     </cfRule>

</xml_diff>